<commit_message>
more cwm tables and figs
</commit_message>
<xml_diff>
--- a/Output tables/CWM_indtraits_ANOVA_all_wide.xlsx
+++ b/Output tables/CWM_indtraits_ANOVA_all_wide.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\McLaughlinSeedBank\Seed_trait_paper_public\Seedbanks_traits_global_change\Output tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4ECB218-2B47-4D6F-AE24-993D470D1E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F68A82-5C37-4491-A1EF-B160873CB6A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F07CCA8A-B80D-4602-A7A4-B33CC7F3532B}"/>
   </bookViews>
@@ -958,7 +958,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:L15"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>